<commit_message>
Product Edit & Order Changes
</commit_message>
<xml_diff>
--- a/backend/importData/bankTable.xlsx
+++ b/backend/importData/bankTable.xlsx
@@ -244,6 +244,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,9 +276,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -585,13 +589,13 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,7 +611,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -627,7 +631,7 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>42034</v>
       </c>
       <c r="F2" t="s">
@@ -647,7 +651,7 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>42034</v>
       </c>
       <c r="F3" t="s">
@@ -667,7 +671,7 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>42034</v>
       </c>
       <c r="F4" t="s">
@@ -687,7 +691,7 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>42034</v>
       </c>
       <c r="F5" t="s">
@@ -707,7 +711,7 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>42034</v>
       </c>
       <c r="F6" t="s">
@@ -727,7 +731,7 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>42034</v>
       </c>
       <c r="F7" t="s">
@@ -747,7 +751,7 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>42034</v>
       </c>
       <c r="F8" t="s">
@@ -767,7 +771,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>42034</v>
       </c>
       <c r="F9" t="s">
@@ -787,7 +791,7 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>42034</v>
       </c>
       <c r="F10" t="s">
@@ -807,7 +811,7 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>42034</v>
       </c>
       <c r="F11" t="s">
@@ -827,7 +831,7 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>42034</v>
       </c>
       <c r="F12" t="s">
@@ -847,7 +851,7 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>42034</v>
       </c>
       <c r="F13" t="s">
@@ -867,7 +871,7 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>42034</v>
       </c>
       <c r="F14" t="s">
@@ -887,7 +891,7 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>42034</v>
       </c>
       <c r="F15" t="s">
@@ -907,7 +911,7 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
         <v>42034</v>
       </c>
       <c r="F16" t="s">
@@ -927,7 +931,7 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>42034</v>
       </c>
       <c r="F17" t="s">
@@ -947,7 +951,7 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>42034</v>
       </c>
       <c r="F18" t="s">
@@ -967,7 +971,7 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>42034</v>
       </c>
       <c r="F19" t="s">
@@ -987,7 +991,7 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
         <v>42034</v>
       </c>
       <c r="F20" t="s">
@@ -1007,7 +1011,7 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>42034</v>
       </c>
       <c r="F21" t="s">
@@ -1027,7 +1031,7 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
         <v>42034</v>
       </c>
       <c r="F22" t="s">
@@ -1047,7 +1051,7 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
         <v>42034</v>
       </c>
       <c r="F23" t="s">
@@ -1067,7 +1071,7 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
         <v>42034</v>
       </c>
       <c r="F24" t="s">
@@ -1087,7 +1091,7 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="2">
         <v>42034</v>
       </c>
       <c r="F25" t="s">
@@ -1107,7 +1111,7 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="2">
         <v>42034</v>
       </c>
       <c r="F26" t="s">
@@ -1127,7 +1131,7 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2">
         <v>42034</v>
       </c>
       <c r="F27" t="s">
@@ -1147,7 +1151,7 @@
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="2">
         <v>42034</v>
       </c>
       <c r="F28" t="s">
@@ -1167,7 +1171,7 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="2">
         <v>42034</v>
       </c>
       <c r="F29" t="s">
@@ -1187,7 +1191,7 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="2">
         <v>42034</v>
       </c>
       <c r="F30" t="s">
@@ -1207,7 +1211,7 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="2">
         <v>42034</v>
       </c>
       <c r="F31" t="s">
@@ -1227,7 +1231,7 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="2">
         <v>42089.665057870399</v>
       </c>
       <c r="F32" t="s">
@@ -1247,7 +1251,7 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
         <v>42091.533807870401</v>
       </c>
       <c r="F33" t="s">
@@ -1267,7 +1271,7 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
         <v>42093</v>
       </c>
       <c r="F34" t="s">
@@ -1276,5 +1280,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>